<commit_message>
Se añaden una parte de los codigo de los programas
</commit_message>
<xml_diff>
--- a/parametros/parametros del sistema.xlsx
+++ b/parametros/parametros del sistema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Github\integradorAnexos\parametros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quiceno\Documents\Git\integradorAnexos\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>Artes integradas</t>
   </si>
@@ -234,13 +234,49 @@
   </si>
   <si>
     <t>Programa</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>SNIES</t>
+  </si>
+  <si>
+    <t>Se añade otras carreras</t>
+  </si>
+  <si>
+    <t>Instituto de Educacion Y Pedagogia</t>
+  </si>
+  <si>
+    <t>Licenciatura en Educacion Popular</t>
+  </si>
+  <si>
+    <t>Licenciatura en Educacion Fisica y Deporte</t>
+  </si>
+  <si>
+    <t>Recreacion</t>
+  </si>
+  <si>
+    <t>Instituto de Psicologia</t>
+  </si>
+  <si>
+    <t>Primera Infancia</t>
+  </si>
+  <si>
+    <t>Nota esta se llama licenciatura en arte dramatica</t>
+  </si>
+  <si>
+    <t>Nota verificar que sea correcto</t>
+  </si>
+  <si>
+    <t>Estudios Politicos Y Resolucion de Conflictos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,13 +284,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -269,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +340,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,367 +628,672 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>3545</v>
+      </c>
+      <c r="D3" s="1">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>3548</v>
+      </c>
+      <c r="D4" s="1">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>3552</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>3556</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C8" s="1">
+        <v>3555</v>
+      </c>
+      <c r="D8" s="1">
+        <v>551</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C10" s="1">
+        <v>3541</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19063</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>3146</v>
+      </c>
+      <c r="D17" s="1">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>3148</v>
+      </c>
+      <c r="D19" s="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>2131</v>
+      </c>
+      <c r="D20" s="1">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>3845</v>
+      </c>
+      <c r="D23" s="1">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>3841</v>
+      </c>
+      <c r="D24" s="1">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>3857</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>2835</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>3647</v>
+      </c>
+      <c r="D30" s="1">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>3645</v>
+      </c>
+      <c r="D31" s="1">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>3646</v>
+      </c>
+      <c r="D32" s="1">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>3648</v>
+      </c>
+      <c r="D33" s="1">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>3661</v>
+      </c>
+      <c r="D35" s="1">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>3651</v>
+      </c>
+      <c r="D36" s="1">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <v>3340</v>
+      </c>
+      <c r="D42" s="1">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="1">
+        <v>3251</v>
+      </c>
+      <c r="D52" s="1">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="1">
+        <v>3249</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
+        <v>3745</v>
+      </c>
+      <c r="D58" s="1">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="1">
+        <v>3747</v>
+      </c>
+      <c r="D59" s="1">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="1">
+        <v>3753</v>
+      </c>
+      <c r="D60" s="1">
+        <v>20261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="1">
+        <v>3741</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2966</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
+        <v>3743</v>
+      </c>
+      <c r="D62" s="1">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="1">
+        <v>3746</v>
+      </c>
+      <c r="D63" s="1">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="1">
+        <v>3744</v>
+      </c>
+      <c r="D64" s="1">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="1">
+        <v>3751</v>
+      </c>
+      <c r="D65" s="1">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="1">
+        <v>3748</v>
+      </c>
+      <c r="D66" s="1">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>3749</v>
+      </c>
+      <c r="D67" s="1">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>3754</v>
+      </c>
+      <c r="D68" s="1">
+        <v>54459</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>3740</v>
+      </c>
+      <c r="D69" s="1">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>2711</v>
+      </c>
+      <c r="D74" s="1">
+        <v>15955</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="1">
+        <v>3489</v>
+      </c>
+      <c r="D79" s="1">
+        <v>16014</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="1">
+        <v>3486</v>
+      </c>
+      <c r="D80" s="1">
+        <v>19058</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" s="1">
+        <v>3490</v>
+      </c>
+      <c r="D81" s="1">
+        <v>106564</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3464</v>
+      </c>
+      <c r="D82" s="1">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>78</v>
+      </c>
+      <c r="C85" s="1">
+        <v>3411</v>
+      </c>
+      <c r="D85" s="1">
+        <v>107492</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A77:D77"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se subrayan los programa que fueron añadidos a la base de datos
</commit_message>
<xml_diff>
--- a/parametros/parametros del sistema.xlsx
+++ b/parametros/parametros del sistema.xlsx
@@ -306,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,13 +347,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,16 +654,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -662,37 +673,40 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>3545</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>591</v>
       </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>3548</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <v>577</v>
       </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>3552</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="7">
         <v>16011</v>
       </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -730,13 +744,14 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>3541</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="7">
         <v>19063</v>
       </c>
     </row>
@@ -766,15 +781,16 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>3146</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="7">
         <v>594</v>
       </c>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -782,26 +798,28 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="7">
         <v>3148</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="7">
         <v>596</v>
       </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="7">
         <v>2131</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="7">
         <v>549</v>
       </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -809,37 +827,40 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="7">
         <v>3845</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="7">
         <v>580</v>
       </c>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="7">
         <v>3841</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="7">
         <v>581</v>
       </c>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="7">
         <v>3857</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="7">
         <v>1953</v>
       </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -863,130 +884,135 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="7">
         <v>3647</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="7">
         <v>565</v>
       </c>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="7">
         <v>3645</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="7">
         <v>566</v>
       </c>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="7">
         <v>3646</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="7">
         <v>568</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="7">
         <v>3648</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="7">
         <v>569</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="7">
         <v>3661</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="7">
         <v>571</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="7">
         <v>3651</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="7">
         <v>572</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="1">
+      <c r="C41" s="7">
         <v>3340</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D41" s="7">
         <v>579</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>42</v>
       </c>
@@ -1007,15 +1033,16 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="B52" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="7">
         <v>3251</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="7">
         <v>555</v>
       </c>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
@@ -1023,12 +1050,13 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="B54" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="7">
         <v>3249</v>
       </c>
+      <c r="D54" s="7"/>
       <c r="E54" t="s">
         <v>80</v>
       </c>
@@ -1044,226 +1072,246 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="B58" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="7">
         <v>3745</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="7">
         <v>582</v>
       </c>
+      <c r="E58" s="6"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="B59" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="7">
         <v>3747</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="7">
         <v>583</v>
       </c>
+      <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="B60" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="7">
         <v>3753</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="7">
         <v>20261</v>
       </c>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="B61" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="7">
         <v>3741</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="7">
         <v>2966</v>
       </c>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="B62" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="7">
         <v>3743</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="7">
         <v>584</v>
       </c>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="B63" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="7">
         <v>3746</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="7">
         <v>585</v>
       </c>
+      <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="B64" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="7">
         <v>3744</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="7">
         <v>586</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="7">
         <v>3751</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="7">
         <v>587</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="7">
         <v>3748</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="7">
         <v>588</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="7">
         <v>3749</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="7">
         <v>589</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="7">
         <v>3754</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="7">
         <v>54459</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="7">
         <v>3740</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="7">
         <v>5004</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="7">
         <v>2712</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="7"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="7">
         <v>2710</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="7"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="7">
         <v>2711</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="7">
         <v>15955</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="6" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="7">
         <v>3489</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="7">
         <v>16014</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="7">
         <v>3486</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="7">
         <v>19058</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="7">
         <v>3490</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="7">
         <v>106564</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>76</v>
       </c>
@@ -1274,21 +1322,22 @@
         <v>576</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="7">
         <v>3411</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="7">
         <v>107492</v>
       </c>
+      <c r="E85" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>